<commit_message>
feat: add test for empty-first-row xlsx file
</commit_message>
<xml_diff>
--- a/tests/file.xlsx
+++ b/tests/file.xlsx
@@ -12,7 +12,7 @@
     <sheet name="REI_1987" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" name="REI_1987" vbProcedure="false">REI_1987!$A$1:$CB$36630</definedName>
+    <definedName function="false" hidden="false" name="REI_1987" vbProcedure="false">REI_1987!$A$2:$CB$36631</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="REI_1987" vbProcedure="false">Notice!$A$1:$B$81</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -316,8 +316,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -346,63 +350,63 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="55.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="55.42"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -499,669 +503,669 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AJ6"/>
+  <dimension ref="A2:AJ7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="2" style="0" width="7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="11" style="0" width="4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="77" min="15" style="0" width="13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="78" min="78" style="0" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="79" min="79" style="0" width="4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="80" min="80" style="0" width="6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="2" style="1" width="7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="1" width="6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="11" style="1" width="4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="77" min="15" style="1" width="13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="78" min="78" style="1" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="79" min="79" style="1" width="4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="80" min="80" style="1" width="6"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="N2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="O1" s="0" t="s">
+      <c r="O2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="P1" s="0" t="s">
+      <c r="P2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="Q1" s="0" t="s">
+      <c r="Q2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="R1" s="0" t="s">
+      <c r="R2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="S1" s="0" t="s">
+      <c r="S2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="T1" s="0" t="s">
+      <c r="T2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="U1" s="0" t="s">
+      <c r="U2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="V1" s="0" t="s">
+      <c r="V2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="W1" s="0" t="s">
+      <c r="W2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="X1" s="0" t="s">
+      <c r="X2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Y1" s="0" t="s">
+      <c r="Y2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="Z1" s="0" t="s">
+      <c r="Z2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AA1" s="0" t="s">
+      <c r="AA2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AB1" s="0" t="s">
+      <c r="AB2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AC1" s="0" t="s">
+      <c r="AC2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AD1" s="0" t="s">
+      <c r="AD2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AE1" s="0" t="s">
+      <c r="AE2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AF1" s="0" t="s">
+      <c r="AF2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AG1" s="0" t="s">
+      <c r="AG2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AH1" s="0" t="s">
+      <c r="AH2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AI1" s="0" t="s">
+      <c r="AI2" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AJ1" s="0" t="s">
+      <c r="AJ2" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E3" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="G3" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="H3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="I3" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="K2" s="0" t="s">
+      <c r="K3" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="L2" s="0" t="s">
+      <c r="L3" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="M2" s="0" t="s">
+      <c r="M3" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="N2" s="0" t="s">
+      <c r="N3" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="O2" s="0" t="n">
+      <c r="O3" s="1" t="n">
         <v>19156</v>
       </c>
-      <c r="P2" s="0" t="n">
+      <c r="P3" s="1" t="n">
         <v>380360</v>
       </c>
-      <c r="Q2" s="0" t="n">
+      <c r="Q3" s="1" t="n">
         <v>123263</v>
       </c>
-      <c r="R2" s="0" t="n">
+      <c r="R3" s="1" t="n">
         <v>5773</v>
       </c>
-      <c r="S2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="T2" s="0" t="n">
+      <c r="S3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="T3" s="1" t="n">
         <v>380360</v>
       </c>
-      <c r="U2" s="0" t="n">
+      <c r="U3" s="1" t="n">
         <v>63975</v>
       </c>
-      <c r="V2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="W2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="X2" s="0" t="n">
+      <c r="V3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X3" s="1" t="n">
         <v>380360</v>
       </c>
-      <c r="Y2" s="0" t="n">
+      <c r="Y3" s="1" t="n">
         <v>7538</v>
       </c>
-      <c r="Z2" s="0" t="n">
+      <c r="Z3" s="1" t="n">
         <v>34395</v>
       </c>
-      <c r="AA2" s="0" t="n">
+      <c r="AA3" s="1" t="n">
         <v>15392</v>
       </c>
-      <c r="AB2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD2" s="0" t="n">
+      <c r="AB3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="1" t="n">
         <v>9959</v>
       </c>
-      <c r="AE2" s="0" t="n">
+      <c r="AE3" s="1" t="n">
         <v>650070</v>
       </c>
-      <c r="AF2" s="0" t="n">
+      <c r="AF3" s="1" t="n">
         <v>54156</v>
       </c>
-      <c r="AG2" s="0" t="n">
+      <c r="AG3" s="1" t="n">
         <v>2522</v>
       </c>
-      <c r="AH2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI2" s="0" t="n">
+      <c r="AH3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI3" s="1" t="n">
         <v>650070</v>
       </c>
-      <c r="AJ2" s="0" t="n">
+      <c r="AJ3" s="1" t="n">
         <v>31138</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D4" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E4" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F4" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="G4" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="H4" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I3" s="0" t="s">
+      <c r="I4" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="K3" s="0" t="s">
+      <c r="K4" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="L3" s="0" t="s">
+      <c r="L4" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="M3" s="0" t="s">
+      <c r="M4" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="N3" s="0" t="s">
+      <c r="N4" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="O3" s="0" t="n">
+      <c r="O4" s="1" t="n">
         <v>1329</v>
       </c>
-      <c r="P3" s="0" t="n">
+      <c r="P4" s="1" t="n">
         <v>42660</v>
       </c>
-      <c r="Q3" s="0" t="n">
+      <c r="Q4" s="1" t="n">
         <v>3867</v>
       </c>
-      <c r="R3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="S3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="T3" s="0" t="n">
+      <c r="R4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="T4" s="1" t="n">
         <v>42660</v>
       </c>
-      <c r="U3" s="0" t="n">
+      <c r="U4" s="1" t="n">
         <v>7172</v>
       </c>
-      <c r="V3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="W3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="X3" s="0" t="n">
+      <c r="V4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X4" s="1" t="n">
         <v>42660</v>
       </c>
-      <c r="Y3" s="0" t="n">
+      <c r="Y4" s="1" t="n">
         <v>839</v>
       </c>
-      <c r="Z3" s="0" t="n">
+      <c r="Z4" s="1" t="n">
         <v>3874</v>
       </c>
-      <c r="AA3" s="0" t="n">
+      <c r="AA4" s="1" t="n">
         <v>1715</v>
       </c>
-      <c r="AB3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD3" s="0" t="n">
+      <c r="AB4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD4" s="1" t="n">
         <v>4639</v>
       </c>
-      <c r="AE3" s="0" t="n">
+      <c r="AE4" s="1" t="n">
         <v>396450</v>
       </c>
-      <c r="AF3" s="0" t="n">
+      <c r="AF4" s="1" t="n">
         <v>39961</v>
       </c>
-      <c r="AG3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI3" s="0" t="n">
+      <c r="AG4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI4" s="1" t="n">
         <v>396450</v>
       </c>
-      <c r="AJ3" s="0" t="n">
+      <c r="AJ4" s="1" t="n">
         <v>18991</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D5" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E5" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="F5" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="G4" s="0" t="s">
+      <c r="G5" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="H4" s="0" t="s">
+      <c r="H5" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I4" s="0" t="s">
+      <c r="I5" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="K4" s="0" t="s">
+      <c r="K5" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="L4" s="0" t="s">
+      <c r="L5" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="M4" s="0" t="s">
+      <c r="M5" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="N4" s="0" t="s">
+      <c r="N5" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="O4" s="0" t="n">
+      <c r="O5" s="1" t="n">
         <v>12153</v>
       </c>
-      <c r="P4" s="0" t="n">
+      <c r="P5" s="1" t="n">
         <v>226910</v>
       </c>
-      <c r="Q4" s="0" t="n">
+      <c r="Q5" s="1" t="n">
         <v>84918</v>
       </c>
-      <c r="R4" s="0" t="n">
+      <c r="R5" s="1" t="n">
         <v>314</v>
       </c>
-      <c r="S4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="T4" s="0" t="n">
+      <c r="S5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="T5" s="1" t="n">
         <v>226910</v>
       </c>
-      <c r="U4" s="0" t="n">
+      <c r="U5" s="1" t="n">
         <v>38176</v>
       </c>
-      <c r="V4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="W4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="X4" s="0" t="n">
+      <c r="V5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X5" s="1" t="n">
         <v>226910</v>
       </c>
-      <c r="Y4" s="0" t="n">
+      <c r="Y5" s="1" t="n">
         <v>4452</v>
       </c>
-      <c r="Z4" s="0" t="n">
+      <c r="Z5" s="1" t="n">
         <v>20672</v>
       </c>
-      <c r="AA4" s="0" t="n">
+      <c r="AA5" s="1" t="n">
         <v>9108</v>
       </c>
-      <c r="AB4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD4" s="0" t="n">
+      <c r="AB5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="1" t="n">
         <v>453053</v>
       </c>
-      <c r="AE4" s="0" t="n">
+      <c r="AE5" s="1" t="n">
         <v>25714770</v>
       </c>
-      <c r="AF4" s="0" t="n">
+      <c r="AF5" s="1" t="n">
         <v>3805800</v>
       </c>
-      <c r="AG4" s="0" t="n">
+      <c r="AG5" s="1" t="n">
         <v>18552</v>
       </c>
-      <c r="AH4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI4" s="0" t="n">
+      <c r="AH5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI5" s="1" t="n">
         <v>25714770</v>
       </c>
-      <c r="AJ4" s="0" t="n">
+      <c r="AJ5" s="1" t="n">
         <v>1231739</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C6" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D6" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E6" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F5" s="0" t="s">
+      <c r="F6" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="G5" s="0" t="s">
+      <c r="G6" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="H5" s="0" t="s">
+      <c r="H6" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I5" s="0" t="s">
+      <c r="I6" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="K5" s="0" t="s">
+      <c r="K6" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="L5" s="0" t="s">
+      <c r="L6" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="M5" s="0" t="s">
+      <c r="M6" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="N5" s="0" t="s">
+      <c r="N6" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="O5" s="0" t="n">
+      <c r="O6" s="1" t="n">
         <v>19973</v>
       </c>
-      <c r="P5" s="0" t="n">
+      <c r="P6" s="1" t="n">
         <v>458340</v>
       </c>
-      <c r="Q5" s="0" t="n">
+      <c r="Q6" s="1" t="n">
         <v>110459</v>
       </c>
-      <c r="R5" s="0" t="n">
+      <c r="R6" s="1" t="n">
         <v>3753</v>
       </c>
-      <c r="S5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="T5" s="0" t="n">
+      <c r="S6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="T6" s="1" t="n">
         <v>458340</v>
       </c>
-      <c r="U5" s="0" t="n">
+      <c r="U6" s="1" t="n">
         <v>77098</v>
       </c>
-      <c r="V5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="W5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="X5" s="0" t="n">
+      <c r="V6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X6" s="1" t="n">
         <v>458340</v>
       </c>
-      <c r="Y5" s="0" t="n">
+      <c r="Y6" s="1" t="n">
         <v>9082</v>
       </c>
-      <c r="Z5" s="0" t="n">
+      <c r="Z6" s="1" t="n">
         <v>41451</v>
       </c>
-      <c r="AA5" s="0" t="n">
+      <c r="AA6" s="1" t="n">
         <v>18553</v>
       </c>
-      <c r="AB5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD5" s="0" t="n">
+      <c r="AB6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD6" s="1" t="n">
         <v>16309</v>
       </c>
-      <c r="AE5" s="0" t="n">
+      <c r="AE6" s="1" t="n">
         <v>1492480</v>
       </c>
-      <c r="AF5" s="0" t="n">
+      <c r="AF6" s="1" t="n">
         <v>131041</v>
       </c>
-      <c r="AG5" s="0" t="n">
+      <c r="AG6" s="1" t="n">
         <v>4465</v>
       </c>
-      <c r="AH5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI5" s="0" t="n">
+      <c r="AH6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI6" s="1" t="n">
         <v>1492480</v>
       </c>
-      <c r="AJ5" s="0" t="n">
+      <c r="AJ6" s="1" t="n">
         <v>71497</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C7" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D7" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E7" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F6" s="0" t="s">
+      <c r="F7" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="G6" s="0" t="s">
+      <c r="G7" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="H6" s="0" t="s">
+      <c r="H7" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I6" s="0" t="s">
+      <c r="I7" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="K6" s="0" t="s">
+      <c r="K7" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="L6" s="0" t="s">
+      <c r="L7" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="M6" s="0" t="s">
+      <c r="M7" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="N6" s="0" t="s">
+      <c r="N7" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="O6" s="0" t="n">
+      <c r="O7" s="1" t="n">
         <v>1995</v>
       </c>
-      <c r="P6" s="0" t="n">
+      <c r="P7" s="1" t="n">
         <v>40250</v>
       </c>
-      <c r="Q6" s="0" t="n">
+      <c r="Q7" s="1" t="n">
         <v>13323</v>
       </c>
-      <c r="R6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="S6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="T6" s="0" t="n">
+      <c r="R7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="T7" s="1" t="n">
         <v>40250</v>
       </c>
-      <c r="U6" s="0" t="n">
+      <c r="U7" s="1" t="n">
         <v>6773</v>
       </c>
-      <c r="V6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="W6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="X6" s="0" t="n">
+      <c r="V7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X7" s="1" t="n">
         <v>40250</v>
       </c>
-      <c r="Y6" s="0" t="n">
+      <c r="Y7" s="1" t="n">
         <v>797</v>
       </c>
-      <c r="Z6" s="0" t="n">
+      <c r="Z7" s="1" t="n">
         <v>3642</v>
       </c>
-      <c r="AA6" s="0" t="n">
+      <c r="AA7" s="1" t="n">
         <v>1626</v>
       </c>
-      <c r="AB6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD6" s="0" t="n">
+      <c r="AB7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD7" s="1" t="n">
         <v>1958</v>
       </c>
-      <c r="AE6" s="0" t="n">
+      <c r="AE7" s="1" t="n">
         <v>163970</v>
       </c>
-      <c r="AF6" s="0" t="n">
+      <c r="AF7" s="1" t="n">
         <v>17101</v>
       </c>
-      <c r="AG6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI6" s="0" t="n">
+      <c r="AG7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI7" s="1" t="n">
         <v>163970</v>
       </c>
-      <c r="AJ6" s="0" t="n">
+      <c r="AJ7" s="1" t="n">
         <v>7859</v>
       </c>
     </row>

</xml_diff>